<commit_message>
Ajuste para do CO_FONTE_SOF ao ivés do CO_FONTE_RECURSO
</commit_message>
<xml_diff>
--- a/FundosBI.xlsx
+++ b/FundosBI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="FAT" sheetId="1" r:id="rId1"/>
@@ -266,10 +266,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -295,10 +309,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,23 +611,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -993,40 +1011,40 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>79018001998.050003</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>27100123081.02</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>293329748.29000002</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>2352298527.9000001</v>
       </c>
       <c r="F9" s="1">
         <v>108763753355.25999</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="4">
         <v>11192064717.700001</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <v>97571688637.559998</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>22181668092.049999</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>40680325821.559998</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="3">
         <v>23564057523.110001</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="3">
         <v>283435904.25999999</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="3">
         <v>86709487340.979996</v>
       </c>
       <c r="N9" s="1">
@@ -1040,40 +1058,40 @@
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>83458886167.919998</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>27136201341.330002</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>663267291.26999998</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>7495294474.0100002</v>
       </c>
       <c r="F10" s="1">
         <v>118753649274.53</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>22402550288.700001</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="3">
         <v>96351098985.830002</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>23274204999.619999</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>47775164661.809998</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="3">
         <v>25020000812</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="3">
         <v>419796121.14999998</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="3">
         <v>96489166594.580002</v>
       </c>
       <c r="N10" s="1">
@@ -1087,40 +1105,40 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>101923163946.50999</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>26345134572.240002</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="3">
         <v>603834237.05999994</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>729664179.16999996</v>
       </c>
       <c r="F11" s="1">
         <v>129601796934.98</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="3">
         <v>21499580680.07</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="3">
         <v>108102216254.91</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="3">
         <v>28361807348.040001</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="3">
         <v>52350535752.720001</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="3">
         <v>28291337053</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="3">
         <v>508369173.05000001</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="3">
         <v>109512049326.81</v>
       </c>
       <c r="N11" s="1">
@@ -1801,14 +1819,14 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -2002,22 +2020,22 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>533832039331.81</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>796693660653.22998</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="5">
         <v>2.6078378274223399</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>763906771440.59998</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>4841921143.5200005</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
         <v>27944968069.110001</v>
       </c>
     </row>
@@ -2025,22 +2043,22 @@
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>588279453204.60999</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>898867275412.72998</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="5">
         <v>2.8381434710634901</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>835137699166.56006</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>7185354602.8500004</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>56544221643.32</v>
       </c>
     </row>
@@ -2048,22 +2066,22 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>639102861155.43994</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>938302029582.81995</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="5">
         <v>2.5475228197379001</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>903643786471.40002</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>8158345375.1999998</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="3">
         <v>26499897736.220001</v>
       </c>
     </row>
@@ -2100,13 +2118,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Z9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.85546875" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Solução CO_FONTE_RECURSO na consulta da despesa
</commit_message>
<xml_diff>
--- a/FundosBI.xlsx
+++ b/FundosBI.xlsx
@@ -612,7 +612,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:H9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,16 +1020,16 @@
       <c r="D9" s="3">
         <v>293329748.29000002</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>2352298527.9000001</v>
       </c>
       <c r="F9" s="1">
         <v>108763753355.25999</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>11192064717.700001</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>97571688637.559998</v>
       </c>
       <c r="I9" s="3">
@@ -1167,7 +1167,7 @@
       <c r="F12" s="1">
         <v>57996940535</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <v>18507889715</v>
       </c>
       <c r="H12" s="1">

</xml_diff>

<commit_message>
Código estavel e valores batendo FAT e RPGP (pequenas diferenças aceitáveis devido a fontes diferentes DW e TG)
</commit_message>
<xml_diff>
--- a/FundosBI.xlsx
+++ b/FundosBI.xlsx
@@ -309,12 +309,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -612,7 +611,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D17" sqref="D17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1166,7 @@
       <c r="F12" s="1">
         <v>57996940535</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>18507889715</v>
       </c>
       <c r="H12" s="1">
@@ -2026,7 +2025,7 @@
       <c r="C9" s="3">
         <v>796693660653.22998</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>2.6078378274223399</v>
       </c>
       <c r="E9" s="3">
@@ -2049,7 +2048,7 @@
       <c r="C10" s="3">
         <v>898867275412.72998</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>2.8381434710634901</v>
       </c>
       <c r="E10" s="3">
@@ -2072,7 +2071,7 @@
       <c r="C11" s="3">
         <v>938302029582.81995</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>2.5475228197379001</v>
       </c>
       <c r="E11" s="3">

</xml_diff>